<commit_message>
removed columns from analysis
</commit_message>
<xml_diff>
--- a/ColumnsUsingAndWhy.xlsx
+++ b/ColumnsUsingAndWhy.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvasquez\Documents\GitHub\CapstoneA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F387E7-6CDA-4BDF-ADFD-0BDD0E52E4E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2C3923-74FD-42DA-961E-5E10238398CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="300" windowWidth="29985" windowHeight="14100" xr2:uid="{0B6F7159-A176-4737-9D48-8C63BC2E22BD}"/>
+    <workbookView xWindow="14100" yWindow="1050" windowWidth="18465" windowHeight="14100" activeTab="1" xr2:uid="{0B6F7159-A176-4737-9D48-8C63BC2E22BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns to use" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="1269">
   <si>
     <t>[WellName]</t>
   </si>
@@ -3217,6 +3218,627 @@
   </si>
   <si>
     <t>Adjusted SQLColumnName</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>UniqueCount</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>AccumulatedFillupStrokes</t>
+  </si>
+  <si>
+    <t>Remove only 1 value in column</t>
+  </si>
+  <si>
+    <t>AccumulatedFillupVolume</t>
+  </si>
+  <si>
+    <t>ADAuxiliary2</t>
+  </si>
+  <si>
+    <t>ADAuxiliary3</t>
+  </si>
+  <si>
+    <t>ADAuxiliary4</t>
+  </si>
+  <si>
+    <t>ADAuxiliary5</t>
+  </si>
+  <si>
+    <t>BitArea</t>
+  </si>
+  <si>
+    <t>BitNozzleTotalFlowArea</t>
+  </si>
+  <si>
+    <t>CoilEngaged</t>
+  </si>
+  <si>
+    <t>CurrentConnectionTime</t>
+  </si>
+  <si>
+    <t>DrillMode</t>
+  </si>
+  <si>
+    <t>DynamicVariable09</t>
+  </si>
+  <si>
+    <t>EC1Active</t>
+  </si>
+  <si>
+    <t>EC1ActivityCode1</t>
+  </si>
+  <si>
+    <t>EC1ActivityCode2</t>
+  </si>
+  <si>
+    <t>EC1ActivityCode3</t>
+  </si>
+  <si>
+    <t>EC1ActivityCode4</t>
+  </si>
+  <si>
+    <t>EC1ActivityCode5</t>
+  </si>
+  <si>
+    <t>EC1Authorized</t>
+  </si>
+  <si>
+    <t>EC1DPModeOn</t>
+  </si>
+  <si>
+    <t>EC1DPModeOnReq</t>
+  </si>
+  <si>
+    <t>EC1DPSPActual</t>
+  </si>
+  <si>
+    <t>EC1DPSPRecommended</t>
+  </si>
+  <si>
+    <t>EC1Ready</t>
+  </si>
+  <si>
+    <t>EC1ROPSPActual</t>
+  </si>
+  <si>
+    <t>EC1ROPSPRecommended</t>
+  </si>
+  <si>
+    <t>EC1WOBModeOn</t>
+  </si>
+  <si>
+    <t>EC1WOBModeOnReq</t>
+  </si>
+  <si>
+    <t>EC1WOBSPActual</t>
+  </si>
+  <si>
+    <t>EC1WOBSPRecommended</t>
+  </si>
+  <si>
+    <t>H2S04</t>
+  </si>
+  <si>
+    <t>H2S08</t>
+  </si>
+  <si>
+    <t>H2S09</t>
+  </si>
+  <si>
+    <t>H2S11</t>
+  </si>
+  <si>
+    <t>HookloadInline</t>
+  </si>
+  <si>
+    <t>LEL01</t>
+  </si>
+  <si>
+    <t>LEL02</t>
+  </si>
+  <si>
+    <t>LEL03</t>
+  </si>
+  <si>
+    <t>LEL05</t>
+  </si>
+  <si>
+    <t>LEL06</t>
+  </si>
+  <si>
+    <t>LEL08</t>
+  </si>
+  <si>
+    <t>LEL09</t>
+  </si>
+  <si>
+    <t>LEL10</t>
+  </si>
+  <si>
+    <t>LEL11</t>
+  </si>
+  <si>
+    <t>LEL12</t>
+  </si>
+  <si>
+    <t>MudMotorRPM</t>
+  </si>
+  <si>
+    <t>OnBottom</t>
+  </si>
+  <si>
+    <t>PLCStatus</t>
+  </si>
+  <si>
+    <t>REVitEnabled</t>
+  </si>
+  <si>
+    <t>REVitUsageAlert</t>
+  </si>
+  <si>
+    <t>ROCKIT_PILOTOnOff</t>
+  </si>
+  <si>
+    <t>SeperatorFlow</t>
+  </si>
+  <si>
+    <t>SlipsSet</t>
+  </si>
+  <si>
+    <t>StaticInjectorForce</t>
+  </si>
+  <si>
+    <t>STCfActualNm_Sec</t>
+  </si>
+  <si>
+    <t>STKfActualNm</t>
+  </si>
+  <si>
+    <t>TDOilSensorBypassAlarm</t>
+  </si>
+  <si>
+    <t>TDOilType</t>
+  </si>
+  <si>
+    <t>TDTorqueInline</t>
+  </si>
+  <si>
+    <t>TongMakeupStartPressure</t>
+  </si>
+  <si>
+    <t>TorqueTare</t>
+  </si>
+  <si>
+    <t>UnderPull</t>
+  </si>
+  <si>
+    <t>VFDVariable10</t>
+  </si>
+  <si>
+    <t>VFDVariable9</t>
+  </si>
+  <si>
+    <t>AccumulatedConnectionTime</t>
+  </si>
+  <si>
+    <t>Removed bc Date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>DateDateOnly</t>
+  </si>
+  <si>
+    <t>DateTimeOnly</t>
+  </si>
+  <si>
+    <t>TripModeAccumulation</t>
+  </si>
+  <si>
+    <t>Removed bc not enough unique values</t>
+  </si>
+  <si>
+    <t>TripModeFillupStrokes</t>
+  </si>
+  <si>
+    <t>ADAutoDrillerRunning</t>
+  </si>
+  <si>
+    <t>ADAuxiliary1</t>
+  </si>
+  <si>
+    <t>ADDifferentialPressureActualValue</t>
+  </si>
+  <si>
+    <t>ADDifferentialPressureLimitValue</t>
+  </si>
+  <si>
+    <t>ADDifferentialPressureSetpointValue</t>
+  </si>
+  <si>
+    <t>ADDPEnabled</t>
+  </si>
+  <si>
+    <t>ADHookloadSlider</t>
+  </si>
+  <si>
+    <t>ADROPActualValue</t>
+  </si>
+  <si>
+    <t>ADROPCruiseControlEnabled</t>
+  </si>
+  <si>
+    <t>ADROPSetpointValue</t>
+  </si>
+  <si>
+    <t>ADSPPSlider</t>
+  </si>
+  <si>
+    <t>ADSystemEnabled</t>
+  </si>
+  <si>
+    <t>ADWOBActualValue</t>
+  </si>
+  <si>
+    <t>ADWOBEnabled</t>
+  </si>
+  <si>
+    <t>ADWOBLimitValue</t>
+  </si>
+  <si>
+    <t>ADWOBSetpointValue</t>
+  </si>
+  <si>
+    <t>BitRPM</t>
+  </si>
+  <si>
+    <t>BitTime_OffBottom</t>
+  </si>
+  <si>
+    <t>BitTime_OnBottom</t>
+  </si>
+  <si>
+    <t>BlockPosition</t>
+  </si>
+  <si>
+    <t>CasingPressure</t>
+  </si>
+  <si>
+    <t>ConnectionCounter</t>
+  </si>
+  <si>
+    <t>Depth_Bit</t>
+  </si>
+  <si>
+    <t>DepthHoleTVD</t>
+  </si>
+  <si>
+    <t>DifferentialPressure</t>
+  </si>
+  <si>
+    <t>DrillCabTDSUTemp</t>
+  </si>
+  <si>
+    <t>DynamicVariable06</t>
+  </si>
+  <si>
+    <t>DynamicVariable10</t>
+  </si>
+  <si>
+    <t>FlowIn</t>
+  </si>
+  <si>
+    <t>GasTotal_units</t>
+  </si>
+  <si>
+    <t>Hookload</t>
+  </si>
+  <si>
+    <t>HookloadString</t>
+  </si>
+  <si>
+    <t>JobPumpVolumeTotal</t>
+  </si>
+  <si>
+    <t>JobStrokesTotal</t>
+  </si>
+  <si>
+    <t>LagDepthGas</t>
+  </si>
+  <si>
+    <t>LEL04</t>
+  </si>
+  <si>
+    <t>LEL07</t>
+  </si>
+  <si>
+    <t>MWDAzimuth</t>
+  </si>
+  <si>
+    <t>MWDContinuousInclination</t>
+  </si>
+  <si>
+    <t>MWDGammaAPI</t>
+  </si>
+  <si>
+    <t>MWDInclination</t>
+  </si>
+  <si>
+    <t>MWDSrvToolfaceAdvisory</t>
+  </si>
+  <si>
+    <t>MWDSrvToolfaceLimits</t>
+  </si>
+  <si>
+    <t>OverPull</t>
+  </si>
+  <si>
+    <t>Pit01Volume</t>
+  </si>
+  <si>
+    <t>Pit02Volume</t>
+  </si>
+  <si>
+    <t>Pit03Volume</t>
+  </si>
+  <si>
+    <t>Pit04Volume</t>
+  </si>
+  <si>
+    <t>Pit05GL</t>
+  </si>
+  <si>
+    <t>Pit06Volume</t>
+  </si>
+  <si>
+    <t>Pit07Volume</t>
+  </si>
+  <si>
+    <t>PitGLActive</t>
+  </si>
+  <si>
+    <t>PitGLCompanyMan</t>
+  </si>
+  <si>
+    <t>PitGLMudLogger</t>
+  </si>
+  <si>
+    <t>PitGLMWD</t>
+  </si>
+  <si>
+    <t>PitGLSignature</t>
+  </si>
+  <si>
+    <t>PitVolumeActive</t>
+  </si>
+  <si>
+    <t>PitVolumeTotal</t>
+  </si>
+  <si>
+    <t>PreviousConnectionTime</t>
+  </si>
+  <si>
+    <t>PumpOffTime</t>
+  </si>
+  <si>
+    <t>PumpOnTime</t>
+  </si>
+  <si>
+    <t>PumpPressure</t>
+  </si>
+  <si>
+    <t>PumpsOn</t>
+  </si>
+  <si>
+    <t>PumpVolumeTotal</t>
+  </si>
+  <si>
+    <t>ReturnFlow</t>
+  </si>
+  <si>
+    <t>ReturnFlowDetected</t>
+  </si>
+  <si>
+    <t>ROCKIT_BearingActualRW</t>
+  </si>
+  <si>
+    <t>ROCKIT_HITRQLeft</t>
+  </si>
+  <si>
+    <t>ROCKIT_HITRQLeftPercent</t>
+  </si>
+  <si>
+    <t>ROCKIT_HITRQRight</t>
+  </si>
+  <si>
+    <t>ROCKIT_HITRQRightPercent</t>
+  </si>
+  <si>
+    <t>ROCKIT_OnOff</t>
+  </si>
+  <si>
+    <t>ROCKIT_OscillationLeftRW</t>
+  </si>
+  <si>
+    <t>ROCKIT_OscillationRightRW</t>
+  </si>
+  <si>
+    <t>ROCKIT_ResultantToolface</t>
+  </si>
+  <si>
+    <t>ROCKIT_RPMRW</t>
+  </si>
+  <si>
+    <t>ROCKIT_ScoreCardRW</t>
+  </si>
+  <si>
+    <t>ROCKIT_SlidetoMDRW</t>
+  </si>
+  <si>
+    <t>ROCKIT_TFtoRW</t>
+  </si>
+  <si>
+    <t>ROP5xDepthhour</t>
+  </si>
+  <si>
+    <t>ROPDepth_StepDepthHour</t>
+  </si>
+  <si>
+    <t>ROPDepthHour</t>
+  </si>
+  <si>
+    <t>ROPMax</t>
+  </si>
+  <si>
+    <t>ROPMinuteDepth</t>
+  </si>
+  <si>
+    <t>ROPTimeDepthHour</t>
+  </si>
+  <si>
+    <t>RotaryRPM</t>
+  </si>
+  <si>
+    <t>RunningSpeedDown</t>
+  </si>
+  <si>
+    <t>RunningSpeedUp</t>
+  </si>
+  <si>
+    <t>SPM1</t>
+  </si>
+  <si>
+    <t>SPM2</t>
+  </si>
+  <si>
+    <t>SPMTotal</t>
+  </si>
+  <si>
+    <t>Strokes1</t>
+  </si>
+  <si>
+    <t>Strokes1CompanyMan</t>
+  </si>
+  <si>
+    <t>Strokes2</t>
+  </si>
+  <si>
+    <t>Strokes2CompanyMan</t>
+  </si>
+  <si>
+    <t>StrokesTotal</t>
+  </si>
+  <si>
+    <t>StrokesTotalCompanyMan</t>
+  </si>
+  <si>
+    <t>StrokesTotalMudLogger</t>
+  </si>
+  <si>
+    <t>TDPLCAlarm1</t>
+  </si>
+  <si>
+    <t>TDPLCAlarm4</t>
+  </si>
+  <si>
+    <t>TDQuillPosition</t>
+  </si>
+  <si>
+    <t>TDS_AmbientTemperature</t>
+  </si>
+  <si>
+    <t>TDS_BrakeTemperature</t>
+  </si>
+  <si>
+    <t>TDS_HPUOilTankTemperature</t>
+  </si>
+  <si>
+    <t>TDS_HydraulicTemperature</t>
+  </si>
+  <si>
+    <t>TDS_LowerBearingTemp</t>
+  </si>
+  <si>
+    <t>TDS_LubeOilAfterFilterPres</t>
+  </si>
+  <si>
+    <t>TDS_LubeOilPressure</t>
+  </si>
+  <si>
+    <t>TDS_LubeOilTemperature</t>
+  </si>
+  <si>
+    <t>TDS_MotorWindingTemperature1</t>
+  </si>
+  <si>
+    <t>TDS_MotorWindingTemperature2</t>
+  </si>
+  <si>
+    <t>TDS_MotorWindingTemperature3ACOnly</t>
+  </si>
+  <si>
+    <t>TDS_OilPressureAcrosstheFilter</t>
+  </si>
+  <si>
+    <t>TDS_UpperBearingTemp</t>
+  </si>
+  <si>
+    <t>TDSRotaryTorqueLimit</t>
+  </si>
+  <si>
+    <t>TonMilesEventCumulative</t>
+  </si>
+  <si>
+    <t>TonMilesMegajoules</t>
+  </si>
+  <si>
+    <t>TopDriveRPM</t>
+  </si>
+  <si>
+    <t>TopDriveRPMCommand</t>
+  </si>
+  <si>
+    <t>TopDriveTorqueCommand</t>
+  </si>
+  <si>
+    <t>TopDriveTorqueft_lbs</t>
+  </si>
+  <si>
+    <t>TorqueDelta</t>
+  </si>
+  <si>
+    <t>TripGL</t>
+  </si>
+  <si>
+    <t>TripGLCompanyMan</t>
+  </si>
+  <si>
+    <t>TripGLSignature</t>
+  </si>
+  <si>
+    <t>TripVolumeActive</t>
+  </si>
+  <si>
+    <t>WeightonBit</t>
+  </si>
+  <si>
+    <t>Syntax for Python</t>
   </si>
 </sst>
 </file>
@@ -3260,7 +3882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3271,6 +3893,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3587,7 +4211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF7E2DB-DB90-466D-926C-3435C6D30811}">
   <dimension ref="A1:J506"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -18159,4 +18783,3892 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B893684-BF91-42E5-8495-C10CCE1DC850}">
+  <dimension ref="A1:G198"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B2" t="str">
+        <f>", '"&amp;A2&amp;"'"</f>
+        <v>, 'AccumulatedFillupStrokes'</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>725789</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B3" t="str">
+        <f>", '"&amp;A3&amp;"'"</f>
+        <v>, 'AccumulatedFillupVolume'</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>702215</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B4" t="str">
+        <f>", '"&amp;A4&amp;"'"</f>
+        <v>, 'ADAuxiliary2'</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>60</v>
+      </c>
+      <c r="E4">
+        <v>725789</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B5" t="str">
+        <f>", '"&amp;A5&amp;"'"</f>
+        <v>, 'ADAuxiliary3'</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>725789</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B6" t="str">
+        <f>", '"&amp;A6&amp;"'"</f>
+        <v>, 'ADAuxiliary4'</v>
+      </c>
+      <c r="C6">
+        <v>256</v>
+      </c>
+      <c r="D6">
+        <v>256</v>
+      </c>
+      <c r="E6">
+        <v>725789</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B7" t="str">
+        <f>", '"&amp;A7&amp;"'"</f>
+        <v>, 'ADAuxiliary5'</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>42</v>
+      </c>
+      <c r="E7">
+        <v>725789</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B8" t="str">
+        <f>", '"&amp;A8&amp;"'"</f>
+        <v>, 'BitArea'</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>725789</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B9" t="str">
+        <f>", '"&amp;A9&amp;"'"</f>
+        <v>, 'BitNozzleTotalFlowArea'</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>725789</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B10" t="str">
+        <f>", '"&amp;A10&amp;"'"</f>
+        <v>, 'CoilEngaged'</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>725789</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B11" t="str">
+        <f>", '"&amp;A11&amp;"'"</f>
+        <v>, 'CurrentConnectionTime'</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>725789</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B12" t="str">
+        <f>", '"&amp;A12&amp;"'"</f>
+        <v>, 'DrillMode'</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>725789</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B13" t="str">
+        <f>", '"&amp;A13&amp;"'"</f>
+        <v>, 'DynamicVariable09'</v>
+      </c>
+      <c r="C13">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>42</v>
+      </c>
+      <c r="E13">
+        <v>725789</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B14" t="str">
+        <f>", '"&amp;A14&amp;"'"</f>
+        <v>, 'EC1Active'</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>725789</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B15" t="str">
+        <f>", '"&amp;A15&amp;"'"</f>
+        <v>, 'EC1ActivityCode1'</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>725789</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B16" t="str">
+        <f>", '"&amp;A16&amp;"'"</f>
+        <v>, 'EC1ActivityCode2'</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>725789</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B17" t="str">
+        <f>", '"&amp;A17&amp;"'"</f>
+        <v>, 'EC1ActivityCode3'</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>725789</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B18" t="str">
+        <f>", '"&amp;A18&amp;"'"</f>
+        <v>, 'EC1ActivityCode4'</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>725789</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B19" t="str">
+        <f>", '"&amp;A19&amp;"'"</f>
+        <v>, 'EC1ActivityCode5'</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>725789</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B20" t="str">
+        <f>", '"&amp;A20&amp;"'"</f>
+        <v>, 'EC1Authorized'</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>725789</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B21" t="str">
+        <f>", '"&amp;A21&amp;"'"</f>
+        <v>, 'EC1DPModeOn'</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>725789</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B22" t="str">
+        <f>", '"&amp;A22&amp;"'"</f>
+        <v>, 'EC1DPModeOnReq'</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>725789</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B23" t="str">
+        <f>", '"&amp;A23&amp;"'"</f>
+        <v>, 'EC1DPSPActual'</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>725789</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B24" t="str">
+        <f>", '"&amp;A24&amp;"'"</f>
+        <v>, 'EC1DPSPRecommended'</v>
+      </c>
+      <c r="C24">
+        <v>385</v>
+      </c>
+      <c r="D24">
+        <v>385</v>
+      </c>
+      <c r="E24">
+        <v>725789</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B25" t="str">
+        <f>", '"&amp;A25&amp;"'"</f>
+        <v>, 'EC1Ready'</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>725789</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B26" t="str">
+        <f>", '"&amp;A26&amp;"'"</f>
+        <v>, 'EC1ROPSPActual'</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>725789</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B27" t="str">
+        <f>", '"&amp;A27&amp;"'"</f>
+        <v>, 'EC1ROPSPRecommended'</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27">
+        <v>725789</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B28" t="str">
+        <f>", '"&amp;A28&amp;"'"</f>
+        <v>, 'EC1WOBModeOn'</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>725789</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B29" t="str">
+        <f>", '"&amp;A29&amp;"'"</f>
+        <v>, 'EC1WOBModeOnReq'</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>725789</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B30" t="str">
+        <f>", '"&amp;A30&amp;"'"</f>
+        <v>, 'EC1WOBSPActual'</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>725789</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B31" t="str">
+        <f>", '"&amp;A31&amp;"'"</f>
+        <v>, 'EC1WOBSPRecommended'</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>14</v>
+      </c>
+      <c r="E31">
+        <v>725789</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" ref="B32:B71" si="0">", '"&amp;A32&amp;"'"</f>
+        <v>, 'H2S04'</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>49.01</v>
+      </c>
+      <c r="E32">
+        <v>725789</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'H2S08'</v>
+      </c>
+      <c r="C33">
+        <v>-440.65</v>
+      </c>
+      <c r="D33">
+        <v>-440.65</v>
+      </c>
+      <c r="E33">
+        <v>725789</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'H2S09'</v>
+      </c>
+      <c r="C34">
+        <v>-4096.46</v>
+      </c>
+      <c r="D34">
+        <v>-4096.46</v>
+      </c>
+      <c r="E34">
+        <v>725789</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'H2S11'</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>52.91</v>
+      </c>
+      <c r="E35">
+        <v>725789</v>
+      </c>
+      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'HookloadInline'</v>
+      </c>
+      <c r="C36">
+        <v>-440.65</v>
+      </c>
+      <c r="D36">
+        <v>-440.65</v>
+      </c>
+      <c r="E36">
+        <v>725789</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL01'</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>725789</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL02'</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>121.45</v>
+      </c>
+      <c r="E38">
+        <v>725789</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL03'</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>725789</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL05'</v>
+      </c>
+      <c r="C40">
+        <v>-440.65</v>
+      </c>
+      <c r="D40">
+        <v>-440.65</v>
+      </c>
+      <c r="E40">
+        <v>725789</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL06'</v>
+      </c>
+      <c r="C41">
+        <v>-4096.46</v>
+      </c>
+      <c r="D41">
+        <v>-4096.46</v>
+      </c>
+      <c r="E41">
+        <v>725789</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL08'</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>725789</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL09'</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>725789</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL10'</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>725789</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL11'</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>118.51</v>
+      </c>
+      <c r="E45">
+        <v>725789</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'LEL12'</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>725789</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'MudMotorRPM'</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>725789</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'OnBottom'</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>725789</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'PLCStatus'</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>725789</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'REVitEnabled'</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>725789</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'REVitUsageAlert'</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>725775</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'ROCKIT_PILOTOnOff'</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>725789</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'SeperatorFlow'</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>118.67</v>
+      </c>
+      <c r="E53">
+        <v>725789</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'SlipsSet'</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>725789</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'StaticInjectorForce'</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>725789</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'STCfActualNm_Sec'</v>
+      </c>
+      <c r="C56">
+        <v>895</v>
+      </c>
+      <c r="D56">
+        <v>895</v>
+      </c>
+      <c r="E56">
+        <v>725789</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'STKfActualNm'</v>
+      </c>
+      <c r="C57">
+        <v>927</v>
+      </c>
+      <c r="D57">
+        <v>927</v>
+      </c>
+      <c r="E57">
+        <v>725789</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'TDOilSensorBypassAlarm'</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>725789</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'TDOilType'</v>
+      </c>
+      <c r="C59">
+        <v>7590</v>
+      </c>
+      <c r="D59">
+        <v>7590</v>
+      </c>
+      <c r="E59">
+        <v>725789</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'TDTorqueInline'</v>
+      </c>
+      <c r="C60">
+        <v>-4096.46</v>
+      </c>
+      <c r="D60">
+        <v>-4096.46</v>
+      </c>
+      <c r="E60">
+        <v>725789</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'TongMakeupStartPressure'</v>
+      </c>
+      <c r="C61">
+        <v>42</v>
+      </c>
+      <c r="D61">
+        <v>42</v>
+      </c>
+      <c r="E61">
+        <v>725789</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'TorqueTare'</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>725777</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'UnderPull'</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>725789</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'VFDVariable10'</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>725789</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'VFDVariable9'</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>725789</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'AccumulatedConnectionTime'</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>36096130000</v>
+      </c>
+      <c r="E66">
+        <v>725789</v>
+      </c>
+      <c r="F66">
+        <v>1577</v>
+      </c>
+      <c r="G66" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'Date'</v>
+      </c>
+      <c r="C67" s="6">
+        <v>43243.866550925923</v>
+      </c>
+      <c r="D67" s="6">
+        <v>43565.328009259261</v>
+      </c>
+      <c r="E67">
+        <v>725789</v>
+      </c>
+      <c r="F67">
+        <v>689600</v>
+      </c>
+      <c r="G67" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'DateDateOnly'</v>
+      </c>
+      <c r="C68" s="6">
+        <v>43243</v>
+      </c>
+      <c r="D68" s="6">
+        <v>43565</v>
+      </c>
+      <c r="E68">
+        <v>725789</v>
+      </c>
+      <c r="F68">
+        <v>158</v>
+      </c>
+      <c r="G68" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'DateTimeOnly'</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0.99988425925925928</v>
+      </c>
+      <c r="E69">
+        <v>725789</v>
+      </c>
+      <c r="F69">
+        <v>8640</v>
+      </c>
+      <c r="G69" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'TripModeAccumulation'</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>5.86</v>
+      </c>
+      <c r="E70">
+        <v>725789</v>
+      </c>
+      <c r="F70">
+        <v>16</v>
+      </c>
+      <c r="G70" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="0"/>
+        <v>, 'TripModeFillupStrokes'</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>75.59</v>
+      </c>
+      <c r="E71">
+        <v>725789</v>
+      </c>
+      <c r="F71">
+        <v>17</v>
+      </c>
+      <c r="G71" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C72">
+        <v>-1</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>725789</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>129.02000000000001</v>
+      </c>
+      <c r="E73">
+        <v>725775</v>
+      </c>
+      <c r="F73">
+        <v>7397</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C74">
+        <v>-4387.07</v>
+      </c>
+      <c r="D74">
+        <v>1685.7</v>
+      </c>
+      <c r="E74">
+        <v>725789</v>
+      </c>
+      <c r="F74">
+        <v>713402</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C75">
+        <v>40</v>
+      </c>
+      <c r="D75">
+        <v>1100</v>
+      </c>
+      <c r="E75">
+        <v>725789</v>
+      </c>
+      <c r="F75">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>850</v>
+      </c>
+      <c r="E76">
+        <v>725789</v>
+      </c>
+      <c r="F76">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C77">
+        <v>-1</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>725789</v>
+      </c>
+      <c r="F77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>10</v>
+      </c>
+      <c r="E78">
+        <v>725789</v>
+      </c>
+      <c r="F78">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>6795.27</v>
+      </c>
+      <c r="E79">
+        <v>725789</v>
+      </c>
+      <c r="F79">
+        <v>671827</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C80">
+        <v>-1</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>725789</v>
+      </c>
+      <c r="F80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>1400</v>
+      </c>
+      <c r="E81">
+        <v>725789</v>
+      </c>
+      <c r="F81">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="E82">
+        <v>725789</v>
+      </c>
+      <c r="F82">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C83">
+        <v>-1</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>725789</v>
+      </c>
+      <c r="F83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C84">
+        <v>-53.75</v>
+      </c>
+      <c r="D84">
+        <v>152.04</v>
+      </c>
+      <c r="E84">
+        <v>725789</v>
+      </c>
+      <c r="F84">
+        <v>625360</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C85">
+        <v>-1</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>725789</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>80</v>
+      </c>
+      <c r="E86">
+        <v>725789</v>
+      </c>
+      <c r="F86">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>75</v>
+      </c>
+      <c r="E87">
+        <v>725789</v>
+      </c>
+      <c r="F87">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>129.02000000000001</v>
+      </c>
+      <c r="E88">
+        <v>725775</v>
+      </c>
+      <c r="F88">
+        <v>7397</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>1735949</v>
+      </c>
+      <c r="E89">
+        <v>725789</v>
+      </c>
+      <c r="F89">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C90">
+        <v>5910.3</v>
+      </c>
+      <c r="D90">
+        <v>9914826</v>
+      </c>
+      <c r="E90">
+        <v>725789</v>
+      </c>
+      <c r="F90">
+        <v>717036</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C91">
+        <v>-40.479999999999997</v>
+      </c>
+      <c r="D91">
+        <v>120.33</v>
+      </c>
+      <c r="E91">
+        <v>725789</v>
+      </c>
+      <c r="F91">
+        <v>595933</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>11854.17</v>
+      </c>
+      <c r="E92">
+        <v>725789</v>
+      </c>
+      <c r="F92">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>342</v>
+      </c>
+      <c r="E93">
+        <v>725789</v>
+      </c>
+      <c r="F93">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>120600</v>
+      </c>
+      <c r="E94">
+        <v>725789</v>
+      </c>
+      <c r="F94">
+        <v>672389</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>120600</v>
+      </c>
+      <c r="E95">
+        <v>725782</v>
+      </c>
+      <c r="F95">
+        <v>670812</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C96">
+        <v>-4387.03</v>
+      </c>
+      <c r="D96">
+        <v>1742.52</v>
+      </c>
+      <c r="E96">
+        <v>725788</v>
+      </c>
+      <c r="F96">
+        <v>704736</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C97">
+        <v>-56.38</v>
+      </c>
+      <c r="D97">
+        <v>323</v>
+      </c>
+      <c r="E97">
+        <v>725789</v>
+      </c>
+      <c r="F97">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>4858.29</v>
+      </c>
+      <c r="E98">
+        <v>725789</v>
+      </c>
+      <c r="F98">
+        <v>689500</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>101.51</v>
+      </c>
+      <c r="E99">
+        <v>725789</v>
+      </c>
+      <c r="F99">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C100">
+        <v>-0.25</v>
+      </c>
+      <c r="D100">
+        <v>795.04</v>
+      </c>
+      <c r="E100">
+        <v>725789</v>
+      </c>
+      <c r="F100">
+        <v>2647</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C101">
+        <v>-106.44</v>
+      </c>
+      <c r="D101">
+        <v>2217.6</v>
+      </c>
+      <c r="E101">
+        <v>725789</v>
+      </c>
+      <c r="F101">
+        <v>85850</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C102">
+        <v>15.93</v>
+      </c>
+      <c r="D102">
+        <v>209.39</v>
+      </c>
+      <c r="E102">
+        <v>725789</v>
+      </c>
+      <c r="F102">
+        <v>3701</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>240.64</v>
+      </c>
+      <c r="E103">
+        <v>725789</v>
+      </c>
+      <c r="F103">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>367646.3</v>
+      </c>
+      <c r="E104">
+        <v>725789</v>
+      </c>
+      <c r="F104">
+        <v>709016</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>4392429</v>
+      </c>
+      <c r="E105">
+        <v>725789</v>
+      </c>
+      <c r="F105">
+        <v>709419</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>16884</v>
+      </c>
+      <c r="E106">
+        <v>725789</v>
+      </c>
+      <c r="F106">
+        <v>22127</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>44.28</v>
+      </c>
+      <c r="E107">
+        <v>725789</v>
+      </c>
+      <c r="F107">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>16999.349999999999</v>
+      </c>
+      <c r="E108">
+        <v>725789</v>
+      </c>
+      <c r="F108">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>364.23</v>
+      </c>
+      <c r="E109">
+        <v>725788</v>
+      </c>
+      <c r="F109">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>135.31</v>
+      </c>
+      <c r="E110">
+        <v>702168</v>
+      </c>
+      <c r="F110">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C111">
+        <v>-12.43</v>
+      </c>
+      <c r="D111">
+        <v>1917.65</v>
+      </c>
+      <c r="E111">
+        <v>713735</v>
+      </c>
+      <c r="F111">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C112">
+        <v>85.05</v>
+      </c>
+      <c r="D112">
+        <v>9082</v>
+      </c>
+      <c r="E112">
+        <v>725789</v>
+      </c>
+      <c r="F112">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>360</v>
+      </c>
+      <c r="E113">
+        <v>725789</v>
+      </c>
+      <c r="F113">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C114">
+        <v>5</v>
+      </c>
+      <c r="D114">
+        <v>45</v>
+      </c>
+      <c r="E114">
+        <v>725789</v>
+      </c>
+      <c r="F114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>21.36</v>
+      </c>
+      <c r="E115">
+        <v>725789</v>
+      </c>
+      <c r="F115">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>93.87</v>
+      </c>
+      <c r="E116">
+        <v>725789</v>
+      </c>
+      <c r="F116">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>118.51</v>
+      </c>
+      <c r="E117">
+        <v>725789</v>
+      </c>
+      <c r="F117">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>100.09</v>
+      </c>
+      <c r="E118">
+        <v>725789</v>
+      </c>
+      <c r="F118">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>237.03</v>
+      </c>
+      <c r="E119">
+        <v>725789</v>
+      </c>
+      <c r="F119">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C120">
+        <v>-118.51</v>
+      </c>
+      <c r="D120">
+        <v>62.93</v>
+      </c>
+      <c r="E120">
+        <v>725789</v>
+      </c>
+      <c r="F120">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C121">
+        <v>0.17</v>
+      </c>
+      <c r="D121">
+        <v>118.51</v>
+      </c>
+      <c r="E121">
+        <v>725789</v>
+      </c>
+      <c r="F121">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>118.51</v>
+      </c>
+      <c r="E122">
+        <v>725789</v>
+      </c>
+      <c r="F122">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C123">
+        <v>-592.57000000000005</v>
+      </c>
+      <c r="D123">
+        <v>209.35</v>
+      </c>
+      <c r="E123">
+        <v>725789</v>
+      </c>
+      <c r="F123">
+        <v>16894</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C124">
+        <v>-592.57000000000005</v>
+      </c>
+      <c r="D124">
+        <v>323.73</v>
+      </c>
+      <c r="E124">
+        <v>725789</v>
+      </c>
+      <c r="F124">
+        <v>52670</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C125">
+        <v>-1027.47</v>
+      </c>
+      <c r="D125">
+        <v>415.08</v>
+      </c>
+      <c r="E125">
+        <v>725789</v>
+      </c>
+      <c r="F125">
+        <v>119580</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C126">
+        <v>-1027.47</v>
+      </c>
+      <c r="D126">
+        <v>415.08</v>
+      </c>
+      <c r="E126">
+        <v>725789</v>
+      </c>
+      <c r="F126">
+        <v>119580</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>3637736000</v>
+      </c>
+      <c r="E127">
+        <v>725789</v>
+      </c>
+      <c r="F127">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>594.28</v>
+      </c>
+      <c r="E128">
+        <v>725789</v>
+      </c>
+      <c r="F128">
+        <v>18365</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>694.32</v>
+      </c>
+      <c r="E129">
+        <v>725789</v>
+      </c>
+      <c r="F129">
+        <v>222423</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>50951.58</v>
+      </c>
+      <c r="E130">
+        <v>725789</v>
+      </c>
+      <c r="F130">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C131">
+        <v>5910.09</v>
+      </c>
+      <c r="D131">
+        <v>4496713</v>
+      </c>
+      <c r="E131">
+        <v>725789</v>
+      </c>
+      <c r="F131">
+        <v>8354</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>10549590</v>
+      </c>
+      <c r="E132">
+        <v>725789</v>
+      </c>
+      <c r="F132">
+        <v>709769</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <v>4747.2</v>
+      </c>
+      <c r="E133">
+        <v>725775</v>
+      </c>
+      <c r="F133">
+        <v>689244</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134">
+        <v>725775</v>
+      </c>
+      <c r="F134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>178214.3</v>
+      </c>
+      <c r="E135">
+        <v>725789</v>
+      </c>
+      <c r="F135">
+        <v>626466</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>100.8</v>
+      </c>
+      <c r="E136">
+        <v>725775</v>
+      </c>
+      <c r="F136">
+        <v>95148</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137">
+        <v>725775</v>
+      </c>
+      <c r="F137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>360</v>
+      </c>
+      <c r="E138">
+        <v>725789</v>
+      </c>
+      <c r="F138">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>18210</v>
+      </c>
+      <c r="E139">
+        <v>725789</v>
+      </c>
+      <c r="F139">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>70.06</v>
+      </c>
+      <c r="E140">
+        <v>725775</v>
+      </c>
+      <c r="F140">
+        <v>6743</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>26000</v>
+      </c>
+      <c r="E141">
+        <v>725789</v>
+      </c>
+      <c r="F141">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>100.06</v>
+      </c>
+      <c r="E142">
+        <v>725775</v>
+      </c>
+      <c r="F142">
+        <v>10202</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>725789</v>
+      </c>
+      <c r="F143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>15</v>
+      </c>
+      <c r="E144">
+        <v>725789</v>
+      </c>
+      <c r="F144">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>33</v>
+      </c>
+      <c r="E145">
+        <v>725789</v>
+      </c>
+      <c r="F145">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>360</v>
+      </c>
+      <c r="E146">
+        <v>725789</v>
+      </c>
+      <c r="F146">
+        <v>3601</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C147">
+        <v>-129</v>
+      </c>
+      <c r="D147">
+        <v>100</v>
+      </c>
+      <c r="E147">
+        <v>725789</v>
+      </c>
+      <c r="F147">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C148">
+        <v>-100</v>
+      </c>
+      <c r="D148">
+        <v>99</v>
+      </c>
+      <c r="E148">
+        <v>725789</v>
+      </c>
+      <c r="F148">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>14630</v>
+      </c>
+      <c r="E149">
+        <v>725789</v>
+      </c>
+      <c r="F149">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>360</v>
+      </c>
+      <c r="E150">
+        <v>725789</v>
+      </c>
+      <c r="F150">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>30291.11</v>
+      </c>
+      <c r="E151">
+        <v>725789</v>
+      </c>
+      <c r="F151">
+        <v>23753</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>568051.80000000005</v>
+      </c>
+      <c r="E152">
+        <v>725784</v>
+      </c>
+      <c r="F152">
+        <v>292389</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>51618.400000000001</v>
+      </c>
+      <c r="E153">
+        <v>725789</v>
+      </c>
+      <c r="F153">
+        <v>465192</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>568051.80000000005</v>
+      </c>
+      <c r="E154">
+        <v>725789</v>
+      </c>
+      <c r="F154">
+        <v>223130</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <v>3493116</v>
+      </c>
+      <c r="E155">
+        <v>725789</v>
+      </c>
+      <c r="F155">
+        <v>218962</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>3867.85</v>
+      </c>
+      <c r="E156">
+        <v>725789</v>
+      </c>
+      <c r="F156">
+        <v>701928</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>129.02000000000001</v>
+      </c>
+      <c r="E157">
+        <v>725775</v>
+      </c>
+      <c r="F157">
+        <v>7397</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>4946.43</v>
+      </c>
+      <c r="E158">
+        <v>725789</v>
+      </c>
+      <c r="F158">
+        <v>300350</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>43.04</v>
+      </c>
+      <c r="E159">
+        <v>725789</v>
+      </c>
+      <c r="F159">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C160">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D160">
+        <v>115.01</v>
+      </c>
+      <c r="E160">
+        <v>725789</v>
+      </c>
+      <c r="F160">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C161">
+        <v>-0.09</v>
+      </c>
+      <c r="D161">
+        <v>115.03</v>
+      </c>
+      <c r="E161">
+        <v>725789</v>
+      </c>
+      <c r="F161">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C162">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D162">
+        <v>200</v>
+      </c>
+      <c r="E162">
+        <v>725789</v>
+      </c>
+      <c r="F162">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>3038754</v>
+      </c>
+      <c r="E163">
+        <v>725789</v>
+      </c>
+      <c r="F163">
+        <v>663354</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164">
+        <v>3734315</v>
+      </c>
+      <c r="E164">
+        <v>725789</v>
+      </c>
+      <c r="F164">
+        <v>662507</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C165">
+        <v>3.91</v>
+      </c>
+      <c r="D165">
+        <v>2106107</v>
+      </c>
+      <c r="E165">
+        <v>725789</v>
+      </c>
+      <c r="F165">
+        <v>668946</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C166">
+        <v>1.75</v>
+      </c>
+      <c r="D166">
+        <v>5809267</v>
+      </c>
+      <c r="E166">
+        <v>725789</v>
+      </c>
+      <c r="F166">
+        <v>669480</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
+      <c r="D167">
+        <v>1787506</v>
+      </c>
+      <c r="E167">
+        <v>725789</v>
+      </c>
+      <c r="F167">
+        <v>599419</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>1977410</v>
+      </c>
+      <c r="E168">
+        <v>725789</v>
+      </c>
+      <c r="F168">
+        <v>710089</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C169">
+        <v>0</v>
+      </c>
+      <c r="D169">
+        <v>4392395</v>
+      </c>
+      <c r="E169">
+        <v>725789</v>
+      </c>
+      <c r="F169">
+        <v>709339</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C170">
+        <v>-2139095000</v>
+      </c>
+      <c r="D170">
+        <v>276824100</v>
+      </c>
+      <c r="E170">
+        <v>725789</v>
+      </c>
+      <c r="F170">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C171">
+        <v>-2147484000</v>
+      </c>
+      <c r="D171">
+        <v>1073873000</v>
+      </c>
+      <c r="E171">
+        <v>725789</v>
+      </c>
+      <c r="F171">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>360</v>
+      </c>
+      <c r="E172">
+        <v>725789</v>
+      </c>
+      <c r="F172">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C173">
+        <v>26.06</v>
+      </c>
+      <c r="D173">
+        <v>113</v>
+      </c>
+      <c r="E173">
+        <v>725789</v>
+      </c>
+      <c r="F173">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C174">
+        <v>31.1</v>
+      </c>
+      <c r="D174">
+        <v>134.06</v>
+      </c>
+      <c r="E174">
+        <v>725789</v>
+      </c>
+      <c r="F174">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C175">
+        <v>-355.56</v>
+      </c>
+      <c r="D175">
+        <v>355.54</v>
+      </c>
+      <c r="E175">
+        <v>725789</v>
+      </c>
+      <c r="F175">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C176">
+        <v>26.6</v>
+      </c>
+      <c r="D176">
+        <v>149.9</v>
+      </c>
+      <c r="E176">
+        <v>725789</v>
+      </c>
+      <c r="F176">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C177">
+        <v>-328</v>
+      </c>
+      <c r="D177">
+        <v>694.98</v>
+      </c>
+      <c r="E177">
+        <v>725789</v>
+      </c>
+      <c r="F177">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>238.1</v>
+      </c>
+      <c r="E178">
+        <v>725789</v>
+      </c>
+      <c r="F178">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>245.7</v>
+      </c>
+      <c r="E179">
+        <v>725789</v>
+      </c>
+      <c r="F179">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C180">
+        <v>33.08</v>
+      </c>
+      <c r="D180">
+        <v>142.52000000000001</v>
+      </c>
+      <c r="E180">
+        <v>725789</v>
+      </c>
+      <c r="F180">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C181">
+        <v>43.16</v>
+      </c>
+      <c r="D181">
+        <v>212.72</v>
+      </c>
+      <c r="E181">
+        <v>725789</v>
+      </c>
+      <c r="F181">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C182">
+        <v>40.1</v>
+      </c>
+      <c r="D182">
+        <v>205.16</v>
+      </c>
+      <c r="E182">
+        <v>725789</v>
+      </c>
+      <c r="F182">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C183">
+        <v>41</v>
+      </c>
+      <c r="D183">
+        <v>204.26</v>
+      </c>
+      <c r="E183">
+        <v>725789</v>
+      </c>
+      <c r="F183">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184">
+        <v>65.37</v>
+      </c>
+      <c r="E184">
+        <v>725789</v>
+      </c>
+      <c r="F184">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C185">
+        <v>40.1</v>
+      </c>
+      <c r="D185">
+        <v>181.04</v>
+      </c>
+      <c r="E185">
+        <v>725789</v>
+      </c>
+      <c r="F185">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C186">
+        <v>9500</v>
+      </c>
+      <c r="D186">
+        <v>27000</v>
+      </c>
+      <c r="E186">
+        <v>725789</v>
+      </c>
+      <c r="F186">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>2698.45</v>
+      </c>
+      <c r="E187">
+        <v>725789</v>
+      </c>
+      <c r="F187">
+        <v>680682</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>3384.84</v>
+      </c>
+      <c r="E188">
+        <v>725789</v>
+      </c>
+      <c r="F188">
+        <v>678223</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>129.02000000000001</v>
+      </c>
+      <c r="E189">
+        <v>725789</v>
+      </c>
+      <c r="F189">
+        <v>7423</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>129.02000000000001</v>
+      </c>
+      <c r="E190">
+        <v>725789</v>
+      </c>
+      <c r="F190">
+        <v>7423</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191">
+        <v>35621.980000000003</v>
+      </c>
+      <c r="E191">
+        <v>725789</v>
+      </c>
+      <c r="F191">
+        <v>20717</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192">
+        <v>35621.980000000003</v>
+      </c>
+      <c r="E192">
+        <v>725789</v>
+      </c>
+      <c r="F192">
+        <v>20717</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>27040.31</v>
+      </c>
+      <c r="E193">
+        <v>725777</v>
+      </c>
+      <c r="F193">
+        <v>20722</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C194">
+        <v>-130.37</v>
+      </c>
+      <c r="D194">
+        <v>85.59</v>
+      </c>
+      <c r="E194">
+        <v>725789</v>
+      </c>
+      <c r="F194">
+        <v>6471</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C195">
+        <v>-143.75</v>
+      </c>
+      <c r="D195">
+        <v>99.29</v>
+      </c>
+      <c r="E195">
+        <v>725789</v>
+      </c>
+      <c r="F195">
+        <v>10488</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>3637738000</v>
+      </c>
+      <c r="E196">
+        <v>725789</v>
+      </c>
+      <c r="F196">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>101.63</v>
+      </c>
+      <c r="E197">
+        <v>725789</v>
+      </c>
+      <c r="F197">
+        <v>4715</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C198">
+        <v>0</v>
+      </c>
+      <c r="D198">
+        <v>167.38</v>
+      </c>
+      <c r="E198">
+        <v>725788</v>
+      </c>
+      <c r="F198">
+        <v>610124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>